<commit_message>
app share by kakao list
</commit_message>
<xml_diff>
--- a/democracyaction/direct_democracy.xlsx
+++ b/democracyaction/direct_democracy.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2764" uniqueCount="2409">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2808" uniqueCount="2441">
   <si>
     <t>name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -7778,7 +7778,112 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>1.0.4</t>
+    <t>office</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1577-7667</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>theminjookr</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>npad_kr</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.youtube.com/user/minjootv</t>
+  </si>
+  <si>
+    <t>http://theminjoo.kr</t>
+  </si>
+  <si>
+    <t>http://blog.naver.com/yesminjoo</t>
+  </si>
+  <si>
+    <t>http://www.libertykoreaparty.kr</t>
+  </si>
+  <si>
+    <t>libertykoreaparty</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/c/%EC%9E%90%EC%9C%A0%ED%95%9C%EA%B5%AD%EB%8B%B9</t>
+  </si>
+  <si>
+    <t>libertykorea</t>
+  </si>
+  <si>
+    <t>http://blog.libertykoreaparty.kr/</t>
+  </si>
+  <si>
+    <t>02-3786-3000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>liberty_kr</t>
+  </si>
+  <si>
+    <t>http://people21.kr</t>
+  </si>
+  <si>
+    <t>saejeongchi0202</t>
+  </si>
+  <si>
+    <t>peopleparty21</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/channel/UCpnetwDnXC5eFlQhjmbv12g</t>
+  </si>
+  <si>
+    <t>http://blog.naver.com/peopleparty21</t>
+  </si>
+  <si>
+    <t>02-715-2000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://bareun.party/</t>
+  </si>
+  <si>
+    <t>02-2070-5600</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bareunpartypage</t>
+  </si>
+  <si>
+    <t>bareunparty</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/channel/UCgg_aa230dghE8hkc7yUXBw</t>
+  </si>
+  <si>
+    <t>http://www.justice21.org</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>justiceKR</t>
+  </si>
+  <si>
+    <t>kr_justice</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/channel/UC4KdOy46f0HCJBqTiq7MLPg</t>
+  </si>
+  <si>
+    <t>http://blog.naver.com/justiceparty</t>
+  </si>
+  <si>
+    <t>jbhyendx</t>
+  </si>
+  <si>
+    <t>02-2038-0103</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.0.5</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -8277,7 +8382,7 @@
   <dimension ref="B2:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -8291,7 +8396,7 @@
         <v>2402</v>
       </c>
       <c r="C2" t="s">
-        <v>2408</v>
+        <v>2440</v>
       </c>
     </row>
     <row r="3" spans="2:3" ht="49.5">
@@ -8307,7 +8412,7 @@
         <v>2404</v>
       </c>
       <c r="C4" s="19">
-        <v>42904</v>
+        <v>42928</v>
       </c>
     </row>
     <row r="5" spans="2:3" ht="132">
@@ -8318,7 +8423,7 @@
         <v>2407</v>
       </c>
     </row>
-    <row r="7" spans="2:3" ht="1.5" hidden="1"/>
+    <row r="7" spans="2:3" hidden="1"/>
     <row r="8" spans="2:3" ht="86.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -8331,9 +8436,9 @@
   <dimension ref="B2:T301"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="990" activePane="bottomLeft"/>
+      <pane ySplit="990" topLeftCell="A282" activePane="bottomLeft"/>
       <selection activeCell="O301" sqref="O301"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomLeft" activeCell="C298" sqref="C298"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -12529,8 +12634,7 @@
         <v>2117</v>
       </c>
       <c r="E106">
-        <f>groups!$B$3</f>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F106" t="s">
         <v>566</v>
@@ -20288,15 +20392,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:D9"/>
+  <dimension ref="B2:O9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
   <sheetData>
-    <row r="2" spans="2:4">
+    <row r="2" spans="2:15">
       <c r="B2" t="s">
         <v>3</v>
       </c>
@@ -20306,48 +20410,180 @@
       <c r="D2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="2:4">
+      <c r="E2" t="s">
+        <v>2408</v>
+      </c>
+      <c r="F2" t="s">
+        <v>246</v>
+      </c>
+      <c r="G2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" t="s">
+        <v>703</v>
+      </c>
+      <c r="K2" t="s">
+        <v>571</v>
+      </c>
+      <c r="L2" t="s">
+        <v>16</v>
+      </c>
+      <c r="M2" t="s">
+        <v>17</v>
+      </c>
+      <c r="N2" t="s">
+        <v>733</v>
+      </c>
+      <c r="O2" t="s">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="3" spans="2:15">
       <c r="B3">
         <v>1</v>
       </c>
       <c r="C3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="2:4">
+      <c r="E3" t="s">
+        <v>2409</v>
+      </c>
+      <c r="G3" t="s">
+        <v>2411</v>
+      </c>
+      <c r="H3" t="s">
+        <v>2410</v>
+      </c>
+      <c r="K3" t="s">
+        <v>2412</v>
+      </c>
+      <c r="L3" t="s">
+        <v>2413</v>
+      </c>
+      <c r="M3" t="s">
+        <v>2414</v>
+      </c>
+    </row>
+    <row r="4" spans="2:15">
       <c r="B4">
         <v>2</v>
       </c>
       <c r="C4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="2:4">
+      <c r="E4" t="s">
+        <v>2420</v>
+      </c>
+      <c r="G4" t="s">
+        <v>2421</v>
+      </c>
+      <c r="H4" t="s">
+        <v>2416</v>
+      </c>
+      <c r="I4" t="s">
+        <v>2418</v>
+      </c>
+      <c r="J4" t="s">
+        <v>2418</v>
+      </c>
+      <c r="K4" t="s">
+        <v>2417</v>
+      </c>
+      <c r="L4" t="s">
+        <v>2415</v>
+      </c>
+      <c r="M4" t="s">
+        <v>2419</v>
+      </c>
+    </row>
+    <row r="5" spans="2:15">
       <c r="B5">
         <v>3</v>
       </c>
       <c r="C5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="2:4">
+      <c r="E5" t="s">
+        <v>2427</v>
+      </c>
+      <c r="G5" t="s">
+        <v>2424</v>
+      </c>
+      <c r="H5" t="s">
+        <v>2423</v>
+      </c>
+      <c r="J5" t="s">
+        <v>2424</v>
+      </c>
+      <c r="K5" t="s">
+        <v>2425</v>
+      </c>
+      <c r="L5" t="s">
+        <v>2422</v>
+      </c>
+      <c r="M5" t="s">
+        <v>2426</v>
+      </c>
+    </row>
+    <row r="6" spans="2:15">
       <c r="B6">
         <v>4</v>
       </c>
       <c r="C6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="2:4">
+      <c r="E6" t="s">
+        <v>2429</v>
+      </c>
+      <c r="G6" t="s">
+        <v>2431</v>
+      </c>
+      <c r="H6" t="s">
+        <v>2430</v>
+      </c>
+      <c r="K6" t="s">
+        <v>2432</v>
+      </c>
+      <c r="L6" t="s">
+        <v>2428</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15">
       <c r="B7">
         <v>5</v>
       </c>
       <c r="C7" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="8" spans="2:4">
+      <c r="E7" t="s">
+        <v>2439</v>
+      </c>
+      <c r="G7" t="s">
+        <v>2435</v>
+      </c>
+      <c r="H7" t="s">
+        <v>2434</v>
+      </c>
+      <c r="I7" t="s">
+        <v>2438</v>
+      </c>
+      <c r="K7" t="s">
+        <v>2436</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>2433</v>
+      </c>
+      <c r="M7" t="s">
+        <v>2437</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15">
       <c r="B8">
         <v>6</v>
       </c>
@@ -20355,7 +20591,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="2:4">
+    <row r="9" spans="2:15">
       <c r="B9">
         <v>7</v>
       </c>
@@ -20365,7 +20601,10 @@
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="L7" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
applies firebase remote config instead of  versions function
</commit_message>
<xml_diff>
--- a/democracyaction/direct_democracy.xlsx
+++ b/democracyaction/direct_democracy.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="19200" windowHeight="11865" tabRatio="699" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="19200" windowHeight="11865" tabRatio="699"/>
   </bookViews>
   <sheets>
     <sheet name="info" sheetId="4" r:id="rId1"/>
@@ -8361,11 +8361,14 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>1.2.2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1. 의원 정보 갱신
+    <t>1.2.3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 의원 정보 화면에 즐겨찾기 버튼 추가
+2. 전면 광고가 활성화되지 않는 문제 수정
+[1.2.2]
+1. 의원 정보 갱신
 2. 의원직 상실, 당적 변경, 정당 해체 반영
 3. 쌍 ㅈ (ㅉ)으로 초성검색되지 않는 문제 수정
 4. 의원 정보에서 사이트 목록의 카페 아이콘 버튼이 동작하지 않는 문제 수정
@@ -8952,7 +8955,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -8983,7 +8986,7 @@
         <v>1993</v>
       </c>
       <c r="C4" s="17">
-        <v>43698</v>
+        <v>43705</v>
       </c>
     </row>
     <row r="5" spans="2:3" ht="198.75" customHeight="1">
@@ -9006,7 +9009,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:V299"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+    <sheetView topLeftCell="H1" workbookViewId="0">
       <pane ySplit="990" topLeftCell="A161" activePane="bottomLeft"/>
       <selection pane="bottomLeft" activeCell="T163" sqref="T163"/>
     </sheetView>

</xml_diff>